<commit_message>
Update  TR-RGR all changes as per review
</commit_message>
<xml_diff>
--- a/DHL/Template/20230322_ TR_SIR_v8.1.xlsx
+++ b/DHL/Template/20230322_ TR_SIR_v8.1.xlsx
@@ -1152,22 +1152,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1186,6 +1171,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1618,10 +1618,10 @@
   <dimension ref="A1:AC46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="7" ySplit="5" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="5" topLeftCell="H45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
+      <selection pane="bottomRight" activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,13 +1655,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,120 +1687,120 @@
       <c r="AB1" s="2"/>
     </row>
     <row r="2" spans="1:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="35" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="35" t="s">
+      <c r="K2" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="35" t="s">
+      <c r="L2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="37" t="s">
+      <c r="P2" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="37" t="s">
+      <c r="Q2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="35" t="s">
+      <c r="R2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="35" t="s">
+      <c r="S2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="T2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="36" t="s">
+      <c r="U2" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="36" t="s">
+      <c r="V2" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="37" t="s">
+      <c r="W2" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="37" t="s">
+      <c r="X2" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="35" t="s">
+      <c r="Y2" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="35" t="s">
+      <c r="Z2" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="35" t="s">
+      <c r="AB2" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="33"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
     </row>
     <row r="4" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1810,48 +1810,48 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35" t="s">
+      <c r="K4" s="31"/>
+      <c r="L4" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35" t="s">
+      <c r="M4" s="31"/>
+      <c r="N4" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="O4" s="35"/>
-      <c r="P4" s="33" t="s">
+      <c r="O4" s="31"/>
+      <c r="P4" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="34"/>
+      <c r="Q4" s="39"/>
       <c r="R4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="S4" s="33" t="s">
+      <c r="S4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="U4" s="31" t="s">
+      <c r="T4" s="39"/>
+      <c r="U4" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="V4" s="32"/>
-      <c r="W4" s="31" t="s">
+      <c r="V4" s="42"/>
+      <c r="W4" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="X4" s="32"/>
+      <c r="X4" s="42"/>
       <c r="Y4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="Z4" s="33" t="s">
+      <c r="Z4" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="34"/>
+      <c r="AA4" s="39"/>
       <c r="AB4" s="4" t="s">
         <v>38</v>
       </c>
@@ -3826,22 +3826,12 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="Z4:AA4"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="J4:K4"/>
@@ -3858,12 +3848,22 @@
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="Z4:AA4"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>